<commit_message>
Added *.xlsx to gitignore
</commit_message>
<xml_diff>
--- a/ProfileUrls.xlsx
+++ b/ProfileUrls.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/naeeramin/Documents/UTS_3rd_semester/ilab2/github_repo/ARDC-Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B685BF1-BDBF-3D45-931B-A5C018C7124A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F358EF8D-3AD7-1248-8BC7-4C84B38A8426}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16140" xr2:uid="{EF4EA40E-8E54-FF42-9FEA-D3979B3FB203}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Profile_Urls</t>
   </si>
@@ -63,12 +63,6 @@
   </si>
   <si>
     <t>Christopher Pyne</t>
-  </si>
-  <si>
-    <t>asd</t>
-  </si>
-  <si>
-    <t>ads</t>
   </si>
 </sst>
 </file>
@@ -420,10 +414,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51ED97CB-C287-1949-8B30-6518B0959988}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="C7" sqref="A5:C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -466,30 +460,6 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" t="s">
-        <v>9</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>